<commit_message>
version 2.0 de la thèse
</commit_message>
<xml_diff>
--- a/CH5. analyses de l'effet Morton/synthèse des cas/synthèse des cas.xlsx
+++ b/CH5. analyses de l'effet Morton/synthèse des cas/synthèse des cas.xlsx
@@ -8,14 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="comparaison" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculs" sheetId="2" r:id="rId2"/>
+    <sheet name="Morton Keogh" sheetId="5" r:id="rId2"/>
+    <sheet name="Faulkner" sheetId="4" r:id="rId3"/>
+    <sheet name="Panara" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Cas</t>
   </si>
@@ -29,16 +31,7 @@
     <t>Module C [T/V]</t>
   </si>
   <si>
-    <t>Dx</t>
-  </si>
-  <si>
-    <t>Um</t>
-  </si>
-  <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>DT</t>
   </si>
   <si>
     <t>indicateur</t>
@@ -64,6 +57,42 @@
   <si>
     <t>Panara et al. W1 10000 rpm</t>
   </si>
+  <si>
+    <t xml:space="preserve">Longueur du palier Lw [m] </t>
+  </si>
+  <si>
+    <t>alpha  [°C-1]</t>
+  </si>
+  <si>
+    <t>m [kg]</t>
+  </si>
+  <si>
+    <t>Distance en porte à faux L [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rayon du palier [m] </t>
+  </si>
+  <si>
+    <t>coefficient C</t>
+  </si>
+  <si>
+    <t>BAC</t>
+  </si>
+  <si>
+    <t>vitesse</t>
+  </si>
+  <si>
+    <t>W3</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
 </sst>
 </file>
 
@@ -72,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,13 +109,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,18 +139,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -274,7 +319,7 @@
                   <c:v>2.2499868191098265E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2</c:v>
+                  <c:v>0.20100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.05</c:v>
@@ -299,11 +344,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="247435320"/>
-        <c:axId val="247438848"/>
+        <c:axId val="152403456"/>
+        <c:axId val="154789816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="247435320"/>
+        <c:axId val="152403456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -343,7 +388,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247438848"/>
+        <c:crossAx val="154789816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -351,7 +396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247438848"/>
+        <c:axId val="154789816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,7 +499,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247435320"/>
+        <c:crossAx val="152403456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -657,7 +702,7 @@
                   <c:v>0.24940663133010915</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12</c:v>
+                  <c:v>0.13500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.13</c:v>
@@ -666,7 +711,7 @@
                   <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,11 +727,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="578273728"/>
-        <c:axId val="578274120"/>
+        <c:axId val="154789424"/>
+        <c:axId val="154791384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="578273728"/>
+        <c:axId val="154789424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,7 +771,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578274120"/>
+        <c:crossAx val="154791384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -734,7 +779,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="578274120"/>
+        <c:axId val="154791384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +882,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578273728"/>
+        <c:crossAx val="154789424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1048,10 +1093,10 @@
                   <c:v>14.872</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>188.71170731707315</c:v>
+                  <c:v>188.71170731707301</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>39.793599999999991</c:v>
+                  <c:v>30.8</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>67.900000000000006</c:v>
@@ -1060,7 +1105,7 @@
                   <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>344</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,11 +1121,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="578274904"/>
-        <c:axId val="578281960"/>
+        <c:axId val="154791776"/>
+        <c:axId val="154790600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="578274904"/>
+        <c:axId val="154791776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1165,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578281960"/>
+        <c:crossAx val="154790600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1128,7 +1173,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="578281960"/>
+        <c:axId val="154790600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350"/>
@@ -1227,7 +1272,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578274904"/>
+        <c:crossAx val="154791776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1431,10 +1476,10 @@
                   <c:v>1.0511800000005485</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0589776986150177</c:v>
+                  <c:v>1.0589776986150168</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95504639999999985</c:v>
+                  <c:v>0.83575800000000011</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.44135000000000008</c:v>
@@ -1443,7 +1488,7 @@
                   <c:v>1.0367999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1008</c:v>
+                  <c:v>0.93800000000000017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1459,11 +1504,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="573518112"/>
-        <c:axId val="573524776"/>
+        <c:axId val="154788640"/>
+        <c:axId val="154790208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="573518112"/>
+        <c:axId val="154788640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,7 +1548,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="573524776"/>
+        <c:crossAx val="154790208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1511,7 +1556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="573524776"/>
+        <c:axId val="154790208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1609,7 +1654,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="573518112"/>
+        <c:crossAx val="154788640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3805,15 +3850,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>344175</xdr:colOff>
+      <xdr:colOff>106050</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>146325</xdr:rowOff>
+      <xdr:rowOff>98700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3969,6 +4014,92 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>113275</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>189486</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="76200"/>
+          <a:ext cx="8200000" cy="8114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>143791</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>522687</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>170530</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6753225" y="334291"/>
+          <a:ext cx="5199462" cy="4027239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -4258,8 +4389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4286,12 +4417,12 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0.46112475633528266</v>
@@ -4310,7 +4441,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0.31004636363636356</v>
@@ -4329,7 +4460,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>2.2499868191098265E-2</v>
@@ -4338,36 +4469,36 @@
         <v>0.24940663133010915</v>
       </c>
       <c r="D4">
-        <v>188.71170731707315</v>
+        <v>188.71170731707301</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4" si="0">B4*C4*D4</f>
-        <v>1.0589776986150177</v>
+        <v>1.0589776986150168</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>0.2</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="C5">
-        <v>0.12</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D5">
-        <v>39.793599999999991</v>
+        <v>30.8</v>
       </c>
       <c r="F5">
         <f>B5*C5*D5</f>
-        <v>0.95504639999999985</v>
+        <v>0.83575800000000011</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0.05</v>
@@ -4387,7 +4518,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0.08</v>
@@ -4405,20 +4536,20 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0.04</v>
       </c>
       <c r="C8">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D8">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="F8">
         <f>B8*C8*D8</f>
-        <v>1.1008</v>
+        <v>0.93800000000000017</v>
       </c>
     </row>
   </sheetData>
@@ -4430,61 +4561,216 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6">
+        <f>B1*B2*B3*B4/B5*1000*1000</f>
+        <v>30.800000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.1E-5</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6">
+        <f>B1*B2*B3*B4/B5*1000*1000</f>
+        <v>188.71170731707321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
       <c r="B2">
-        <f>0.9*0.0001*1000000</f>
-        <v>90</v>
-      </c>
-      <c r="C2" s="3">
-        <v>454</v>
-      </c>
-      <c r="D2" s="4">
-        <f>B2/C2</f>
-        <v>0.19823788546255505</v>
+        <v>12400</v>
+      </c>
+      <c r="C2">
+        <v>1.05</v>
+      </c>
+      <c r="D2">
+        <v>0.08</v>
+      </c>
+      <c r="E2">
+        <f>C2/D2/F2</f>
+        <v>9.1145833333333329E-2</v>
+      </c>
+      <c r="F2">
+        <v>144</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>10.4</v>
-      </c>
-      <c r="C4">
-        <f>0.9*0.0001*1000000</f>
-        <v>90</v>
-      </c>
-      <c r="D4">
-        <f>B4/C4</f>
-        <v>0.11555555555555556</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3">
+        <v>0.95</v>
+      </c>
+      <c r="D3">
+        <v>0.04</v>
+      </c>
+      <c r="E3">
+        <f>C3/D3/F3</f>
+        <v>7.0895522388059698E-2</v>
+      </c>
+      <c r="F3">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>